<commit_message>
Completa 5-8 y 5.9
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/VIOLENCIA/Hechos_Delictivos/Muertes_Violentas_de_Mujeres_relacionadas_con_hechos_delictivos_2018-2022.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/VIOLENCIA/Hechos_Delictivos/Muertes_Violentas_de_Mujeres_relacionadas_con_hechos_delictivos_2018-2022.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F40A05-DA71-4F2E-B951-A640D2AC97A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105670DA-F857-4FC5-910E-81B51FD10AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="915" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="915" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Índice" sheetId="96" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H21" sqref="H21"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6:G16"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AB41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H21" sqref="H21"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6:G15"/>
@@ -2296,7 +2296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153812CB-9CC5-4368-AEEF-8049A9DAD59E}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>